<commit_message>
Finish the calculation procedure, add background information
</commit_message>
<xml_diff>
--- a/data/calculation.xlsx
+++ b/data/calculation.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">核素</t>
   </si>
@@ -29,6 +29,138 @@
   </si>
   <si>
     <t xml:space="preserve">发射几率</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">本底计数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(630keV-690keV)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">本底计数时长</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(s)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">模拟半球型室内体积</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(m3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">活度浓度设置</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Bq/m3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">模拟时长</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(s)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">全能峰计数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(&gt;630keV)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">总事件数</t>
+  </si>
+  <si>
+    <t xml:space="preserve">探测效率</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">探测限</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Bq/m3, HJ1149)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Cs-137</t>
@@ -110,13 +242,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -136,15 +272,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.56"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -154,22 +296,147 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>661.65</v>
       </c>
+      <c r="C2" s="2" t="n">
+        <v>0.8998</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>4979</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>3718.76635</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <f aca="false">2/3*3.1415926*5^3</f>
+        <v>261.799383333333</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>3200</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>3572</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>97390244</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <f aca="false">I2/J2</f>
+        <v>3.66771850371378E-005</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <f aca="false">4.66*1*SQRT($D2)/($H2*$F2*K2*$C2)</f>
+        <v>11.8931363283846</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="0" t="n">
+        <v>386</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>9742134</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <f aca="false">I3/J3</f>
+        <v>3.96217091655689E-005</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <f aca="false">4.66*1*SQRT($D2)/($H2*$F2*K3*$C2)</f>
+        <v>11.0092868524493</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="E2:E7"/>
+    <mergeCell ref="F2:F7"/>
+    <mergeCell ref="H2:H7"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12页 &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Arial,标准"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,标准"页 &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>